<commit_message>
update table with new bottom offset
</commit_message>
<xml_diff>
--- a/inst/supporting_files/necsc_thermal_metrics_core_outputs.xlsx
+++ b/inst/supporting_files/necsc_thermal_metrics_core_outputs.xlsx
@@ -165,18 +165,9 @@
     <t>bottom temperature at stratification</t>
   </si>
   <si>
-    <t>water temperature 1m from lake bottom on day of stratification (as defined in original stratification measure)</t>
-  </si>
-  <si>
-    <t>mean of bottom temperature (1 m from bottom) from July, August, September</t>
-  </si>
-  <si>
     <t>Max summer bottom temperature</t>
   </si>
   <si>
-    <t>max of bottom temperature (1 m from bottom) from July, August, September</t>
-  </si>
-  <si>
     <t>Mean  summer bottom temperature</t>
   </si>
   <si>
@@ -331,6 +322,15 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>water temperature 0.1m from lake bottom on day of stratification (as defined in original stratification measure)</t>
+  </si>
+  <si>
+    <t>mean of bottom temperature (0.1 m from bottom) from July, August, September</t>
+  </si>
+  <si>
+    <t>max of bottom temperature (0.1 m from bottom) from July, August, September</t>
   </si>
 </sst>
 </file>
@@ -722,7 +722,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -759,12 +759,12 @@
         <v>19</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>23</v>
@@ -773,7 +773,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
@@ -783,12 +783,12 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
@@ -797,7 +797,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>36</v>
@@ -807,12 +807,12 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>23</v>
@@ -821,7 +821,7 @@
         <v>35</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>37</v>
@@ -831,7 +831,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>15</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
@@ -866,7 +866,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
@@ -878,12 +878,12 @@
         <v>16</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
@@ -892,7 +892,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
@@ -904,12 +904,12 @@
         <v>16</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
@@ -918,7 +918,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -926,12 +926,12 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
@@ -940,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
@@ -952,12 +952,12 @@
         <v>16</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -966,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>3</v>
@@ -978,12 +978,12 @@
         <v>16</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
@@ -992,7 +992,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
@@ -1016,7 +1016,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>31</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
@@ -1038,7 +1038,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>32</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
@@ -1061,7 +1061,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>33</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>40</v>
@@ -1084,82 +1084,82 @@
         <v>41</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>11</v>
@@ -1170,19 +1170,19 @@
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>11</v>
@@ -1191,19 +1191,19 @@
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>11</v>
@@ -1212,19 +1212,19 @@
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -1233,19 +1233,19 @@
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>11</v>
@@ -1254,19 +1254,19 @@
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>11</v>
@@ -1275,19 +1275,19 @@
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>11</v>

</xml_diff>